<commit_message>
Added local properties and effective laminate properties to output excel
</commit_message>
<xml_diff>
--- a/Final Project/Case Study Data/case3.xlsx
+++ b/Final Project/Case Study Data/case3.xlsx
@@ -13,7 +13,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+  <si>
+    <t>NxTot</t>
+  </si>
+  <si>
+    <t>NyTot</t>
+  </si>
+  <si>
+    <t>NxyTot</t>
+  </si>
+  <si>
+    <t>Ply</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>Midplane Deformation</t>
+  </si>
+  <si>
+    <t>eps0x</t>
+  </si>
+  <si>
+    <t>eps0y</t>
+  </si>
+  <si>
+    <t>eps0xy</t>
+  </si>
+  <si>
+    <t>Global Stress</t>
+  </si>
+  <si>
+    <t>sigma1</t>
+  </si>
+  <si>
+    <t>sigma2</t>
+  </si>
+  <si>
+    <t>sigma12</t>
+  </si>
+  <si>
+    <t>Global Strain</t>
+  </si>
+  <si>
+    <t>epsilon1</t>
+  </si>
+  <si>
+    <t>epsilon2</t>
+  </si>
+  <si>
+    <t>gamma12</t>
+  </si>
+  <si>
+    <t>MxTot</t>
+  </si>
+  <si>
+    <t>MyTot</t>
+  </si>
+  <si>
+    <t>MxyTot</t>
+  </si>
+  <si>
+    <t>kx</t>
+  </si>
+  <si>
+    <t>ky</t>
+  </si>
+  <si>
+    <t>kxy</t>
+  </si>
+  <si>
+    <t>DeltaT</t>
+  </si>
   <si>
     <t>NxTot</t>
   </si>
@@ -105,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -114,13 +186,15 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -147,21 +221,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" s="0">
         <v>829.65806826558526</v>
       </c>
       <c r="C1" s="0"/>
       <c r="D1" s="0" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="E1" s="0">
         <v>0</v>
       </c>
       <c r="F1" s="0"/>
       <c r="G1" s="0" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="H1" s="0">
         <v>-450</v>
@@ -171,14 +245,14 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0">
         <v>-170.34193173441474</v>
       </c>
       <c r="C2" s="0"/>
       <c r="D2" s="0" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E2" s="0">
         <v>0</v>
@@ -191,14 +265,14 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0">
         <v>2.4980018054066022e-14</v>
       </c>
       <c r="C3" s="0"/>
       <c r="D3" s="0" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="E3" s="0">
         <v>0</v>
@@ -223,7 +297,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0">
         <v>1</v>
@@ -255,7 +329,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B6" s="0">
         <v>-0.02</v>
@@ -299,7 +373,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0"/>
@@ -313,14 +387,14 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B9" s="0">
         <v>0.0031298277647945406</v>
       </c>
       <c r="C9" s="0"/>
       <c r="D9" s="0" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="E9" s="0">
         <v>9.774755977538807e-35</v>
@@ -333,14 +407,14 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B10" s="0">
         <v>-0.00090878954396307046</v>
       </c>
       <c r="C10" s="0"/>
       <c r="D10" s="0" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="E10" s="0">
         <v>5.4228149378825262e-35</v>
@@ -353,14 +427,14 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B11" s="0">
         <v>-2.6105912990350568e-19</v>
       </c>
       <c r="C11" s="0"/>
       <c r="D11" s="0" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E11" s="0">
         <v>-6.3888867485851463e-34</v>
@@ -385,7 +459,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B13" s="0"/>
       <c r="C13" s="0"/>
@@ -399,7 +473,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B14" s="0">
         <v>16538.617308757606</v>
@@ -431,7 +505,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0">
         <v>8461.3826912423829</v>
@@ -463,7 +537,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B16" s="0">
         <v>983.45999105945702</v>
@@ -507,7 +581,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
@@ -521,7 +595,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B19" s="0">
         <v>0.0060139918238021409</v>
@@ -553,7 +627,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B20" s="0">
         <v>0.0019753745150445281</v>
@@ -585,7 +659,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B21" s="0">
         <v>-0.0069749999999999986</v>

</xml_diff>